<commit_message>
added session 1 results
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7810019A-743D-4351-AC5A-A7A5722605B5}"/>
+  <xr:revisionPtr revIDLastSave="383" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E25E1F9-EF7F-4898-BBAF-076E3AA6ACD7}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="55">
   <si>
     <t>manler</t>
   </si>
@@ -194,6 +194,18 @@
   </si>
   <si>
     <t>Et Haneen</t>
+  </si>
+  <si>
+    <t>Down to be on 2nd</t>
+  </si>
+  <si>
+    <t>Interested in 2nd</t>
+  </si>
+  <si>
+    <t>Handy Manny</t>
+  </si>
+  <si>
+    <t>Peethan</t>
   </si>
 </sst>
 </file>
@@ -292,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -314,11 +326,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -334,6 +359,31 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
         </patternFill>
       </fill>
     </dxf>
@@ -704,7 +754,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -735,10 +785,12 @@
       <c r="G1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1"/>
+      <c r="H1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
@@ -749,9 +801,9 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C2" s="4">
         <f>IF(OR(B3 = "UNPLAYED", B3 = "XXX"), B3, -1* B3)</f>
-        <v>UNPLAYED</v>
+        <v>100</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
@@ -773,7 +825,10 @@
         <f>IF(OR(B8 = "UNPLAYED", B8 = "XXX"), B8, -1* B8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="str">
+        <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -781,8 +836,8 @@
       <c r="A3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+      <c r="B3" s="3">
+        <v>-100</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -807,7 +862,10 @@
         <f>IF(OR(C8 = "UNPLAYED", C8 = "XXX"), C8, -1* C8)</f>
         <v>XXX</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="str">
+        <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -840,7 +898,10 @@
         <f>IF(OR(D8 = "UNPLAYED", D8 = "XXX"), D8, -1* D8)</f>
         <v>XXX</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="str">
+        <f>IF(OR(D9 = "UNPLAYED", D9 = "XXX"), D9, -1* D9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -872,7 +933,10 @@
         <f>IF(OR(E8 = "UNPLAYED", E8 = "XXX"), E8, -1* E8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
+        <v>-30</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -903,7 +967,10 @@
         <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="str">
+        <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -933,13 +1000,16 @@
         <f>IF(OR(G8 = "UNPLAYED", G8 = "XXX"), G8, -1* G8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="str">
+        <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -962,20 +1032,41 @@
       <c r="H8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="4" t="str">
+        <f>IF(OR(H9 = "UNPLAYED", H9 = "XXX"), H9, -1* H9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
@@ -1019,11 +1110,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1035,12 +1134,13 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="2" width="12.5234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1065,10 +1165,12 @@
       <c r="G1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1"/>
+      <c r="H1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
@@ -1103,7 +1205,10 @@
         <f>IF(OR(B8 = "UNPLAYED", B8 = "XXX"), B8, -1* B8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="str">
+        <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -1137,7 +1242,10 @@
         <f>IF(OR(C8 = "UNPLAYED", C8 = "XXX"), C8, -1* C8)</f>
         <v>XXX</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="str">
+        <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
@@ -1170,7 +1278,10 @@
         <f>IF(OR(D8 = "UNPLAYED", D8 = "XXX"), D8, -1* D8)</f>
         <v>XXX</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="str">
+        <f>IF(OR(D9 = "UNPLAYED", D9 = "XXX"), D9, -1* D9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
@@ -1202,7 +1313,10 @@
         <f>IF(OR(E8 = "UNPLAYED", E8 = "XXX"), E8, -1* E8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="str">
+        <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -1233,7 +1347,10 @@
         <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="str">
+        <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
@@ -1263,13 +1380,16 @@
         <f>IF(OR(G8 = "UNPLAYED", G8 = "XXX"), G8, -1* G8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="str">
+        <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1292,22 +1412,43 @@
       <c r="H8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="str">
+        <f>IF(OR(H9 = "UNPLAYED", H9 = "XXX"), H9, -1* H9)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+    <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1365,10 +1506,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1381,7 +1530,7 @@
   <dimension ref="A1:O74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1503,8 +1652,8 @@
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="11" t="s">
-        <v>49</v>
+      <c r="A8" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>16</v>
@@ -1519,8 +1668,15 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -2618,7 +2774,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:H8"/>
+      <selection activeCell="I1" sqref="I1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3087,10 +3243,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEB8592-A874-463A-9311-9DED4CF77908}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3213,9 +3369,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="7"/>
-      <c r="M5" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3268,15 +3422,15 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="H8" s="7">
         <v>1</v>
@@ -3291,15 +3445,11 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="H9" s="7">
         <v>1.5</v>
       </c>
@@ -3309,14 +3459,17 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="7"/>
       <c r="B10" s="10" t="s">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="H10" s="7">
         <v>1.5</v>
       </c>
@@ -3329,10 +3482,10 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7"/>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="7"/>
       <c r="H11" s="7">
@@ -3350,7 +3503,7 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7"/>
       <c r="B12" s="11" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C12" s="7"/>
       <c r="H12" s="12">
@@ -3362,24 +3515,25 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="M12" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
beginning of updating me page
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="383" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E25E1F9-EF7F-4898-BBAF-076E3AA6ACD7}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D233F61-E1C3-4FF6-9F69-6CAECDD2E913}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="55">
   <si>
     <t>manler</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Vedant</t>
   </si>
   <si>
+    <t>Anish</t>
+  </si>
+  <si>
     <t>Sam</t>
   </si>
   <si>
@@ -97,9 +100,6 @@
     <t>Ethan</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Hethan</t>
   </si>
   <si>
@@ -196,9 +196,6 @@
     <t>Et Haneen</t>
   </si>
   <si>
-    <t>Down to be on 2nd</t>
-  </si>
-  <si>
     <t>Interested in 2nd</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>Peethan</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>24</v>
@@ -786,10 +786,10 @@
         <v>42</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -1118,10 +1118,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1145,7 +1145,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>24</v>
@@ -1166,10 +1166,10 @@
         <v>42</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -1506,18 +1506,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1529,7 +1529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F4B8BC-1389-42AE-87D2-D523A6E6AA2A}">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1541,7 +1541,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>5</v>
@@ -1576,10 +1576,10 @@
         <v>50</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7"/>
       <c r="L3" s="7"/>
@@ -1592,7 +1592,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>20</v>
@@ -1640,10 +1640,10 @@
         <v>42</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>11</v>
       </c>
       <c r="D7" s="7"/>
       <c r="L7" s="7"/>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7"/>
       <c r="L8" s="7"/>
@@ -1669,13 +1669,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="7"/>
       <c r="L9" s="7"/>
@@ -2784,7 +2784,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>24</v>
@@ -3243,17 +3243,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEB8592-A874-463A-9311-9DED4CF77908}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>5</v>
@@ -3292,7 +3292,7 @@
         <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -3304,10 +3304,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="7">
         <v>1</v>
@@ -3328,7 +3328,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>20</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="5" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="10" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -3363,7 +3363,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>29</v>
@@ -3403,16 +3403,16 @@
         <v>42</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>11</v>
       </c>
       <c r="H7" s="7">
         <v>2</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>43</v>
@@ -3422,15 +3422,15 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="7">
         <v>1</v>
@@ -3445,36 +3445,38 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13"/>
+      <c r="A9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="H9" s="7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="7"/>
       <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="C10" s="13"/>
       <c r="H10" s="7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -3482,28 +3484,30 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="7"/>
-      <c r="B11" s="11" t="s">
-        <v>8</v>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="7"/>
       <c r="H11" s="7">
         <v>1.5</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="M11" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7"/>
       <c r="B12" s="11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C12" s="7"/>
       <c r="H12" s="12">
@@ -3516,24 +3520,34 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated for week 3
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D233F61-E1C3-4FF6-9F69-6CAECDD2E913}"/>
+  <xr:revisionPtr revIDLastSave="431" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15F69DA0-F055-448F-A9E4-362A54A41E4B}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="57">
   <si>
     <t>manler</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>TRON</t>
+  </si>
+  <si>
+    <t>Katy</t>
   </si>
 </sst>
 </file>
@@ -213,7 +219,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -257,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -300,6 +306,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -318,21 +333,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -402,17 +417,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDCD094"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -751,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -767,35 +771,39 @@
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="5" t="s">
         <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -829,11 +837,17 @@
         <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="J2" s="1" t="str">
+        <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="3">
@@ -866,11 +880,17 @@
         <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="1" t="str">
+        <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>IF(OR(C11 = "UNPLAYED", C11 = "XXX"), C11, -1* C11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -886,9 +906,9 @@
         <f>IF(OR(D5 = "UNPLAYED", D5 = "XXX"), D5, -1* D5)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="F4" s="4" t="str">
+      <c r="F4" s="4">
         <f>IF(OR(D6 = "UNPLAYED", D6 = "XXX"), D6, -1* D6)</f>
-        <v>UNPLAYED</v>
+        <v>-100</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>IF(OR(D7 = "UNPLAYED", D7 = "XXX"), D7, -1* D7)</f>
@@ -902,11 +922,17 @@
         <f>IF(OR(D9 = "UNPLAYED", D9 = "XXX"), D9, -1* D9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="1" t="str">
+        <f>IF(OR(D10 = "UNPLAYED", D10 = "XXX"), D10, -1* D10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f>IF(OR(D11 = "UNPLAYED", D11 = "XXX"), D11, -1* D11)</f>
+        <v>XXX</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -937,11 +963,17 @@
         <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
         <v>-30</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1" t="str">
+        <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
+        <v>XXX</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -950,8 +982,8 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
+      <c r="D6" s="3">
+        <v>100</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>4</v>
@@ -959,9 +991,9 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="G6" s="4">
         <f>IF(OR(F7 = "UNPLAYED", F7 = "XXX"), F7, -1* F7)</f>
-        <v>UNPLAYED</v>
+        <v>-40</v>
       </c>
       <c r="H6" s="4" t="str">
         <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
@@ -971,11 +1003,17 @@
         <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="J6" s="1" t="str">
+        <f>IF(OR(F10 = "UNPLAYED", F10 = "XXX"), F10, -1* F10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f>IF(OR(F11 = "UNPLAYED", F11 = "XXX"), F11, -1* F11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -990,8 +1028,8 @@
       <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
+      <c r="F7" s="3">
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>3</v>
@@ -1004,8 +1042,14 @@
         <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1">
+        <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
+        <v>-20</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
@@ -1036,8 +1080,14 @@
         <f>IF(OR(H9 = "UNPLAYED", H9 = "XXX"), H9, -1* H9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="4" t="str">
+        <f>IF(OR(H10 = "UNPLAYED", H10 = "XXX"), H10, -1* H10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f>IF(OR(H11 = "UNPLAYED", H11 = "XXX"), H11, -1* H11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
@@ -1067,34 +1117,85 @@
       <c r="I9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="J9" s="4" t="str">
+        <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K9" s="4" t="str">
+        <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
+        <v>UNPLAYED</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>20</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="4">
+        <f>IF(OR(J11 = "UNPLAYED", J11 = "XXX"), J11, -1* J11)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3">
+        <v>-100</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="1"/>
@@ -1108,20 +1209,23 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:H8">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1134,7 +1238,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1147,35 +1251,39 @@
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="5" t="s">
         <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1189,9 +1297,9 @@
         <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E2" s="1">
         <f>IF(OR(B5 = "UNPLAYED", B5 = "XXX"), B5, -1* B5)</f>
-        <v>UNPLAYED</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>IF(OR(B6 = "UNPLAYED", B6 = "XXX"), B6, -1* B6)</f>
@@ -1209,11 +1317,17 @@
         <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="J2" s="1" t="str">
+        <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1246,11 +1360,17 @@
         <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="1" t="str">
+        <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f>IF(OR(C11 = "UNPLAYED", C11 = "XXX"), C11, -1* C11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1282,15 +1402,21 @@
         <f>IF(OR(D9 = "UNPLAYED", D9 = "XXX"), D9, -1* D9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="1" t="str">
+        <f>IF(OR(D10 = "UNPLAYED", D10 = "XXX"), D10, -1* D10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f>IF(OR(D11 = "UNPLAYED", D11 = "XXX"), D11, -1* D11)</f>
+        <v>XXX</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
+      <c r="B5" s="3">
+        <v>-100</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -1317,11 +1443,17 @@
         <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1">
+        <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
+        <v>-100</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
+        <v>XXX</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1351,11 +1483,17 @@
         <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="J6" s="1" t="str">
+        <f>IF(OR(F10 = "UNPLAYED", F10 = "XXX"), F10, -1* F10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f>IF(OR(F11 = "UNPLAYED", F11 = "XXX"), F11, -1* F11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1384,8 +1522,14 @@
         <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1" t="str">
+        <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
@@ -1416,8 +1560,14 @@
         <f>IF(OR(H9 = "UNPLAYED", H9 = "XXX"), H9, -1* H9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="1"/>
+      <c r="J8" s="4" t="str">
+        <f>IF(OR(H10 = "UNPLAYED", H10 = "XXX"), H10, -1* H10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f>IF(OR(H11 = "UNPLAYED", H11 = "XXX"), H11, -1* H11)</f>
+        <v>UNPLAYED</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
@@ -1447,36 +1597,87 @@
       <c r="I9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="4" t="str">
+        <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
+        <v>UNPLAYED</v>
+      </c>
+      <c r="K9" s="4" t="str">
+        <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+    <row r="10" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>100</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="4" t="str">
+        <f>IF(OR(J11 = "UNPLAYED", J11 = "XXX"), J11, -1* J11)</f>
+        <v>UNPLAYED</v>
+      </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+    <row r="11" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1505,19 +1706,19 @@
       <c r="K13" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:H8">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1527,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F4B8BC-1389-42AE-87D2-D523A6E6AA2A}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1539,7 +1740,7 @@
     <col min="7" max="7" width="7.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -1549,1220 +1750,116 @@
       <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="10" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="10" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="11" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="7"/>
-      <c r="N61" s="7"/>
-      <c r="O61" s="7"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="7"/>
-      <c r="N62" s="7"/>
-      <c r="O62" s="7"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="7"/>
-      <c r="N63" s="7"/>
-      <c r="O63" s="7"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-      <c r="I64" s="7"/>
-      <c r="J64" s="7"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="7"/>
-      <c r="M64" s="7"/>
-      <c r="N64" s="7"/>
-      <c r="O64" s="7"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="7"/>
-      <c r="N65" s="7"/>
-      <c r="O65" s="7"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="7"/>
-      <c r="O66" s="7"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="7"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="7"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="7"/>
-      <c r="N68" s="7"/>
-      <c r="O68" s="7"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
-      <c r="O71" s="7"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
-      <c r="J74" s="7"/>
-      <c r="K74" s="7"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="7"/>
-      <c r="N74" s="7"/>
-      <c r="O74" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2774,7 +1871,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2786,25 +1883,25 @@
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -2818,7 +1915,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2862,7 +1959,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2905,7 +2002,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2947,7 +2044,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2988,7 +2085,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -3028,7 +2125,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -3067,7 +2164,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3243,15 +2340,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEB8592-A874-463A-9311-9DED4CF77908}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3261,55 +2358,47 @@
       <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="10" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -3318,22 +2407,18 @@
       <c r="J3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="10" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4">
         <v>1.5</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -3342,24 +2427,21 @@
       <c r="J4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
       <c r="M4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -3368,21 +2450,18 @@
       <c r="J5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6">
         <v>1.5</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -3391,24 +2470,21 @@
       <c r="J6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7" t="s">
+      <c r="M6" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="11" t="s">
+    </row>
+    <row r="7" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7">
         <v>2</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -3417,135 +2493,99 @@
       <c r="J7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="11" t="s">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="11" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9">
         <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10" t="s">
+    </row>
+    <row r="10" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="H10" s="7">
+      <c r="C10" s="12"/>
+      <c r="H10">
         <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10" t="s">
+    </row>
+    <row r="11" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="H11" s="7">
+      <c r="H11">
         <v>1.5</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7" t="s">
+      <c r="M11" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="7"/>
-      <c r="B12" s="11" t="s">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>1.5</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7" t="s">
+      <c r="M12" t="s">
         <v>51</v>
       </c>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="11" t="s">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="11" t="s">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3655,7 +2695,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C6:C7" si="2">B7 * (B7 - 1) /2 * 2</f>
+        <f t="shared" ref="C7" si="2">B7 * (B7 - 1) /2 * 2</f>
         <v>30</v>
       </c>
       <c r="D7">

</xml_diff>

<commit_message>
updated for the most recent session
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="431" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15F69DA0-F055-448F-A9E4-362A54A41E4B}"/>
+  <xr:revisionPtr revIDLastSave="433" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BF3ABB-E64A-49C2-BD66-DB6D1A5FF51C}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="57">
   <si>
     <t>manler</t>
   </si>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -855,9 +855,9 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="4">
         <f>IF(OR(C4 = "UNPLAYED", C4 = "XXX"), C4, -1* C4)</f>
-        <v>UNPLAYED</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>IF(OR(C5 = "UNPLAYED", C5 = "XXX"), C5, -1* C5)</f>
@@ -895,8 +895,8 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
+      <c r="C4" s="3">
+        <v>-60</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EF8B2E-F019-48DD-B57E-84981A9F67DB}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1288,9 +1288,9 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C2" s="4">
         <f>IF(OR(B3 = "UNPLAYED", B3 = "XXX"), B3, -1* B3)</f>
-        <v>UNPLAYED</v>
+        <v>100</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
@@ -1329,8 +1329,8 @@
       <c r="A3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+      <c r="B3" s="3">
+        <v>-100</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
updated for the post thanksgiving session
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="431" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15F69DA0-F055-448F-A9E4-362A54A41E4B}"/>
+  <xr:revisionPtr revIDLastSave="433" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BF3ABB-E64A-49C2-BD66-DB6D1A5FF51C}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="57">
   <si>
     <t>manler</t>
   </si>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -855,9 +855,9 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="4">
         <f>IF(OR(C4 = "UNPLAYED", C4 = "XXX"), C4, -1* C4)</f>
-        <v>UNPLAYED</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>IF(OR(C5 = "UNPLAYED", C5 = "XXX"), C5, -1* C5)</f>
@@ -895,8 +895,8 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
+      <c r="C4" s="3">
+        <v>-60</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EF8B2E-F019-48DD-B57E-84981A9F67DB}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1288,9 +1288,9 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C2" s="4">
         <f>IF(OR(B3 = "UNPLAYED", B3 = "XXX"), B3, -1* B3)</f>
-        <v>UNPLAYED</v>
+        <v>100</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
@@ -1329,8 +1329,8 @@
       <c r="A3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+      <c r="B3" s="3">
+        <v>-100</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
found bug in number of remaining games
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="433" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BF3ABB-E64A-49C2-BD66-DB6D1A5FF51C}"/>
+  <xr:revisionPtr revIDLastSave="536" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27D64BBE-6643-4120-BDC9-FE67B6E94C8F}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
     <sheet name="AwayGames" sheetId="2" r:id="rId2"/>
-    <sheet name="TeamInfo" sheetId="3" r:id="rId3"/>
-    <sheet name="AwayGamesBig" sheetId="6" r:id="rId4"/>
-    <sheet name="notes" sheetId="5" r:id="rId5"/>
-    <sheet name="GameCalculator" sheetId="4" r:id="rId6"/>
+    <sheet name="Disallowed games" sheetId="7" r:id="rId3"/>
+    <sheet name="TeamInfo" sheetId="3" r:id="rId4"/>
+    <sheet name="AwayGamesBig" sheetId="6" r:id="rId5"/>
+    <sheet name="notes" sheetId="5" r:id="rId6"/>
+    <sheet name="GameCalculator" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="69">
   <si>
     <t>manler</t>
   </si>
@@ -212,6 +213,42 @@
   </si>
   <si>
     <t>Katy</t>
+  </si>
+  <si>
+    <t>count top</t>
+  </si>
+  <si>
+    <t>count left</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>base counts</t>
+  </si>
+  <si>
+    <t>added no games</t>
+  </si>
+  <si>
+    <t>team 1</t>
+  </si>
+  <si>
+    <t>team 2</t>
+  </si>
+  <si>
+    <t>Crok Messiers</t>
+  </si>
+  <si>
+    <t>^ there is a 3 way no overlap. Could make it so you just play each of them once and your result in the series is determined by those 2 ^</t>
+  </si>
+  <si>
+    <t>Doesn't work because then there is also J&amp;J left over</t>
+  </si>
+  <si>
+    <t>way play</t>
+  </si>
+  <si>
+    <t>away TRON won by 100</t>
   </si>
 </sst>
 </file>
@@ -346,7 +383,151 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -757,7 +938,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -838,7 +1019,7 @@
       </c>
       <c r="J2" s="1" t="str">
         <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
@@ -877,7 +1058,7 @@
       </c>
       <c r="I3" s="1" t="str">
         <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
@@ -948,7 +1129,7 @@
       </c>
       <c r="F5" s="4" t="str">
         <f>IF(OR(E6 = "UNPLAYED", E6 = "XXX"), E6, -1* E6)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>IF(OR(E7 = "UNPLAYED", E7 = "XXX"), E7, -1* E7)</f>
@@ -964,11 +1145,11 @@
       </c>
       <c r="J5" s="1" t="str">
         <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="K5" s="1" t="str">
         <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
-        <v>XXX</v>
+        <v>UNPLAYED</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
@@ -984,8 +1165,8 @@
       <c r="D6" s="3">
         <v>100</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>3</v>
@@ -1039,7 +1220,7 @@
       </c>
       <c r="I7" s="4" t="str">
         <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J7" s="1">
         <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
@@ -1047,7 +1228,7 @@
       </c>
       <c r="K7" s="1" t="str">
         <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -1095,8 +1276,8 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
@@ -1107,8 +1288,8 @@
       <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
+      <c r="G9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>4</v>
@@ -1129,8 +1310,8 @@
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1138,8 +1319,8 @@
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>4</v>
@@ -1174,14 +1355,14 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>3</v>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
@@ -1213,18 +1394,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="B2:H5 B8:H8 B6:D7 F6:H7">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1237,7 +1450,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1318,7 +1531,7 @@
       </c>
       <c r="J2" s="1" t="str">
         <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
@@ -1357,7 +1570,7 @@
       </c>
       <c r="I3" s="1" t="str">
         <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
@@ -1428,7 +1641,7 @@
       </c>
       <c r="F5" s="4" t="str">
         <f>IF(OR(E6 = "UNPLAYED", E6 = "XXX"), E6, -1* E6)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>IF(OR(E7 = "UNPLAYED", E7 = "XXX"), E7, -1* E7)</f>
@@ -1442,13 +1655,13 @@
         <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="1" t="str">
         <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
-        <v>-100</v>
+        <v>XXX</v>
       </c>
       <c r="K5" s="1" t="str">
         <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
-        <v>XXX</v>
+        <v>UNPLAYED</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
@@ -1464,8 +1677,8 @@
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>3</v>
@@ -1519,7 +1732,7 @@
       </c>
       <c r="I7" s="4" t="str">
         <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J7" s="1" t="str">
         <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
@@ -1527,7 +1740,7 @@
       </c>
       <c r="K7" s="1" t="str">
         <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -1575,8 +1788,8 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
@@ -1587,8 +1800,8 @@
       <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
+      <c r="G9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>4</v>
@@ -1610,8 +1823,8 @@
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1619,8 +1832,8 @@
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3">
-        <v>100</v>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>4</v>
@@ -1656,14 +1869,14 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>3</v>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
@@ -1706,18 +1919,50 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="B2:H5 B8:H8 B6:D7 F6:H7">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1726,6 +1971,395 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F9ABF2-F401-4C44-99C9-20C25E7AB746}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="6" max="6" width="12.5234375" customWidth="1"/>
+    <col min="8" max="8" width="11.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF(AwayGames!B2:B11, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>B2 + C2</f>
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIF(AwayGames!C3:C12, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(AwayGames!$B3:B3, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>B3 + C3</f>
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF(AwayGames!D4:D13, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF(AwayGames!$B4:C4, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>B4 + C4</f>
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(AwayGames!E5:E14, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(AwayGames!$B5:D5, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>B5 + C5</f>
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF(AwayGames!F6:F15, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIF(AwayGames!$B6:E6, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>B6 + C6</f>
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIF(AwayGames!G7:G16, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>COUNTIF(AwayGames!$B7:F7, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>B7 + C7</f>
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <f>COUNTIF(AwayGames!H8:H17, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>COUNTIF(AwayGames!$B8:G8, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f>B8 + C8</f>
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <f>COUNTIF(AwayGames!I9:I18, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIF(AwayGames!$B9:H9, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f>B9 + C9</f>
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <f>COUNTIF(AwayGames!J10:J19, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(AwayGames!$B10:I10, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>B10 + C10</f>
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <f>COUNTIF(AwayGames!K11:K20, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(AwayGames!$B11:J11, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f>B11 + C11</f>
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="N13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F4B8BC-1389-42AE-87D2-D523A6E6AA2A}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1865,7 +2499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF409A10-1081-455E-AFC1-5E5397C1A5B5}">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -2337,7 +2971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEB8592-A874-463A-9311-9DED4CF77908}">
   <dimension ref="A1:M15"/>
   <sheetViews>
@@ -2593,7 +3227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E89C9DF-CBF0-44E0-B9C4-2CFC23F872E2}">
   <dimension ref="A1:F7"/>
   <sheetViews>

</xml_diff>

<commit_message>
began the game finder with its counts
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27D64BBE-6643-4120-BDC9-FE67B6E94C8F}"/>
+  <xr:revisionPtr revIDLastSave="537" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4AE47CA-5998-468A-B38C-CF24612AABF3}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
@@ -245,7 +245,7 @@
     <t>Doesn't work because then there is also J&amp;J left over</t>
   </si>
   <si>
-    <t>way play</t>
+    <t>was played</t>
   </si>
   <si>
     <t>away TRON won by 100</t>
@@ -1975,7 +1975,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
updated excel file from jpFlicks
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="433" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BF3ABB-E64A-49C2-BD66-DB6D1A5FF51C}"/>
+  <xr:revisionPtr revIDLastSave="540" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFF0F175-4C48-4B9D-B2A4-8A7204FBBC37}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
     <sheet name="AwayGames" sheetId="2" r:id="rId2"/>
-    <sheet name="TeamInfo" sheetId="3" r:id="rId3"/>
-    <sheet name="AwayGamesBig" sheetId="6" r:id="rId4"/>
-    <sheet name="notes" sheetId="5" r:id="rId5"/>
-    <sheet name="GameCalculator" sheetId="4" r:id="rId6"/>
+    <sheet name="Disallowed games" sheetId="7" r:id="rId3"/>
+    <sheet name="TeamInfo" sheetId="3" r:id="rId4"/>
+    <sheet name="AwayGamesBig" sheetId="6" r:id="rId5"/>
+    <sheet name="notes" sheetId="5" r:id="rId6"/>
+    <sheet name="GameCalculator" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="69">
   <si>
     <t>manler</t>
   </si>
@@ -212,6 +213,42 @@
   </si>
   <si>
     <t>Katy</t>
+  </si>
+  <si>
+    <t>count top</t>
+  </si>
+  <si>
+    <t>count left</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>base counts</t>
+  </si>
+  <si>
+    <t>added no games</t>
+  </si>
+  <si>
+    <t>team 1</t>
+  </si>
+  <si>
+    <t>team 2</t>
+  </si>
+  <si>
+    <t>Crok Messiers</t>
+  </si>
+  <si>
+    <t>^ there is a 3 way no overlap. Could make it so you just play each of them once and your result in the series is determined by those 2 ^</t>
+  </si>
+  <si>
+    <t>Doesn't work because then there is also J&amp;J left over</t>
+  </si>
+  <si>
+    <t>was played</t>
+  </si>
+  <si>
+    <t>away TRON won by 100</t>
   </si>
 </sst>
 </file>
@@ -346,7 +383,115 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCD094"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -435,6 +580,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -757,7 +906,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -824,9 +973,9 @@
         <f>IF(OR(B6 = "UNPLAYED", B6 = "XXX"), B6, -1* B6)</f>
         <v>XXX</v>
       </c>
-      <c r="G2" s="1" t="str">
+      <c r="G2" s="1">
         <f>IF(OR(B7 = "UNPLAYED", B7 = "XXX"), B7, -1* B7)</f>
-        <v>UNPLAYED</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="str">
         <f>IF(OR(B8 = "UNPLAYED", B8 = "XXX"), B8, -1* B8)</f>
@@ -838,7 +987,7 @@
       </c>
       <c r="J2" s="1" t="str">
         <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
@@ -877,7 +1026,7 @@
       </c>
       <c r="I3" s="1" t="str">
         <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
@@ -948,7 +1097,7 @@
       </c>
       <c r="F5" s="4" t="str">
         <f>IF(OR(E6 = "UNPLAYED", E6 = "XXX"), E6, -1* E6)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>IF(OR(E7 = "UNPLAYED", E7 = "XXX"), E7, -1* E7)</f>
@@ -964,11 +1113,11 @@
       </c>
       <c r="J5" s="1" t="str">
         <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="K5" s="1" t="str">
         <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
-        <v>XXX</v>
+        <v>UNPLAYED</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
@@ -984,8 +1133,8 @@
       <c r="D6" s="3">
         <v>100</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>3</v>
@@ -994,9 +1143,9 @@
         <f>IF(OR(F7 = "UNPLAYED", F7 = "XXX"), F7, -1* F7)</f>
         <v>-40</v>
       </c>
-      <c r="H6" s="4" t="str">
+      <c r="H6" s="4">
         <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
-        <v>UNPLAYED</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1" t="str">
         <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
@@ -1015,8 +1164,8 @@
       <c r="A7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
+      <c r="B7" s="3">
+        <v>-10</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
@@ -1033,13 +1182,13 @@
       <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="4" t="str">
+      <c r="H7" s="4">
         <f>IF(OR(G8 = "UNPLAYED", G8 = "XXX"), G8, -1* G8)</f>
-        <v>UNPLAYED</v>
+        <v>75</v>
       </c>
       <c r="I7" s="4" t="str">
         <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J7" s="1">
         <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
@@ -1047,7 +1196,7 @@
       </c>
       <c r="K7" s="1" t="str">
         <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -1066,11 +1215,11 @@
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>4</v>
+      <c r="F8" s="3">
+        <v>-100</v>
+      </c>
+      <c r="G8" s="3">
+        <v>-75</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>3</v>
@@ -1095,8 +1244,8 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
@@ -1107,8 +1256,8 @@
       <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
+      <c r="G9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>4</v>
@@ -1129,8 +1278,8 @@
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1138,8 +1287,8 @@
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>4</v>
@@ -1174,14 +1323,14 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>3</v>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
@@ -1212,19 +1361,43 @@
       <c r="K13" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <conditionalFormatting sqref="B9:B10">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="B2:H5 B6:D7 F6:H7 B8:H8">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1237,7 +1410,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1318,7 +1491,7 @@
       </c>
       <c r="J2" s="1" t="str">
         <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>IF(OR(B11 = "UNPLAYED", B11 = "XXX"), B11, -1* B11)</f>
@@ -1357,7 +1530,7 @@
       </c>
       <c r="I3" s="1" t="str">
         <f>IF(OR(C9 = "UNPLAYED", C9 = "XXX"), C9, -1* C9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J3" s="1" t="str">
         <f>IF(OR(C10 = "UNPLAYED", C10 = "XXX"), C10, -1* C10)</f>
@@ -1428,7 +1601,7 @@
       </c>
       <c r="F5" s="4" t="str">
         <f>IF(OR(E6 = "UNPLAYED", E6 = "XXX"), E6, -1* E6)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>IF(OR(E7 = "UNPLAYED", E7 = "XXX"), E7, -1* E7)</f>
@@ -1442,13 +1615,13 @@
         <f>IF(OR(E9 = "UNPLAYED", E9 = "XXX"), E9, -1* E9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="1" t="str">
         <f>IF(OR(E10 = "UNPLAYED", E10 = "XXX"), E10, -1* E10)</f>
-        <v>-100</v>
+        <v>XXX</v>
       </c>
       <c r="K5" s="1" t="str">
         <f>IF(OR(E11 = "UNPLAYED", E11 = "XXX"), E11, -1* E11)</f>
-        <v>XXX</v>
+        <v>UNPLAYED</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="25.8" thickBot="1" x14ac:dyDescent="0.6">
@@ -1464,8 +1637,8 @@
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>3</v>
@@ -1519,7 +1692,7 @@
       </c>
       <c r="I7" s="4" t="str">
         <f>IF(OR(G9 = "UNPLAYED", G9 = "XXX"), G9, -1* G9)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
       <c r="J7" s="1" t="str">
         <f>IF(OR(G10 = "UNPLAYED", G10 = "XXX"), G10, -1* G10)</f>
@@ -1527,7 +1700,7 @@
       </c>
       <c r="K7" s="1" t="str">
         <f>IF(OR(G11 = "UNPLAYED", G11 = "XXX"), G11, -1* G11)</f>
-        <v>UNPLAYED</v>
+        <v>XXX</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -1575,8 +1748,8 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
@@ -1587,8 +1760,8 @@
       <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>4</v>
+      <c r="G9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>4</v>
@@ -1610,8 +1783,8 @@
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -1619,8 +1792,8 @@
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3">
-        <v>100</v>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>4</v>
@@ -1656,14 +1829,14 @@
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>3</v>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
@@ -1705,19 +1878,43 @@
       <c r="K13" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="B9:B10">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:H8">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="B2:H5 B6:D7 F6:H7 B8:H8">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"UNPLAYED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"XXX"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"UNPLAYED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"XXX"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1726,6 +1923,395 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F9ABF2-F401-4C44-99C9-20C25E7AB746}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="6" max="6" width="12.5234375" customWidth="1"/>
+    <col min="8" max="8" width="11.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF(AwayGames!B2:B11, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D11" si="0">B2 + C2</f>
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIF(AwayGames!C3:C12, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(AwayGames!$B3:B3, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF(AwayGames!D4:D13, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF(AwayGames!$B4:C4, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(AwayGames!E5:E14, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(AwayGames!$B5:D5, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF(AwayGames!F6:F15, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIF(AwayGames!$B6:E6, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIF(AwayGames!G7:G16, "XXX")</f>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>COUNTIF(AwayGames!$B7:F7, "XXX")</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <f>COUNTIF(AwayGames!H8:H17, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>COUNTIF(AwayGames!$B8:G8, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <f>COUNTIF(AwayGames!I9:I18, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIF(AwayGames!$B9:H9, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <f>COUNTIF(AwayGames!J10:J19, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(AwayGames!$B10:I10, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <f>COUNTIF(AwayGames!K11:K20, "XXX")</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(AwayGames!$B11:J11, "XXX")</f>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="N13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F4B8BC-1389-42AE-87D2-D523A6E6AA2A}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1865,7 +2451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF409A10-1081-455E-AFC1-5E5397C1A5B5}">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -2337,7 +2923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEB8592-A874-463A-9311-9DED4CF77908}">
   <dimension ref="A1:M15"/>
   <sheetViews>
@@ -2593,7 +3179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E89C9DF-CBF0-44E0-B9C4-2CFC23F872E2}">
   <dimension ref="A1:F7"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated for the 15th results
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="540" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFF0F175-4C48-4B9D-B2A4-8A7204FBBC37}"/>
+  <xr:revisionPtr revIDLastSave="544" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47FC00E8-1281-4563-94C4-CA62B8F806BC}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="69">
   <si>
     <t>manler</t>
   </si>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -965,9 +965,9 @@
         <f>IF(OR(B4 = "UNPLAYED", B4 = "XXX"), B4, -1* B4)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E2" s="1">
         <f>IF(OR(B5 = "UNPLAYED", B5 = "XXX"), B5, -1* B5)</f>
-        <v>UNPLAYED</v>
+        <v>95</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>IF(OR(B6 = "UNPLAYED", B6 = "XXX"), B6, -1* B6)</f>
@@ -1012,9 +1012,9 @@
         <f>IF(OR(C5 = "UNPLAYED", C5 = "XXX"), C5, -1* C5)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="F3" s="1" t="str">
+      <c r="F3" s="1">
         <f>IF(OR(C6 = "UNPLAYED", C6 = "XXX"), C6, -1* C6)</f>
-        <v>UNPLAYED</v>
+        <v>-55</v>
       </c>
       <c r="G3" s="1" t="str">
         <f>IF(OR(C7 = "UNPLAYED", C7 = "XXX"), C7, -1* C7)</f>
@@ -1083,8 +1083,8 @@
       <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
+      <c r="B5" s="3">
+        <v>-95</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -1127,8 +1127,8 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
+      <c r="C6" s="3">
+        <v>55</v>
       </c>
       <c r="D6" s="3">
         <v>100</v>
@@ -1269,9 +1269,9 @@
         <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="K9" s="4" t="str">
+      <c r="K9" s="4">
         <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
-        <v>UNPLAYED</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.55000000000000004">
@@ -1335,8 +1335,8 @@
       <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>4</v>
+      <c r="I11" s="3">
+        <v>-15</v>
       </c>
       <c r="J11" s="3">
         <v>-100</v>
@@ -1409,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EF8B2E-F019-48DD-B57E-84981A9F67DB}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1643,9 +1643,9 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="str">
+      <c r="G6" s="4">
         <f>IF(OR(F7 = "UNPLAYED", F7 = "XXX"), F7, -1* F7)</f>
-        <v>UNPLAYED</v>
+        <v>45</v>
       </c>
       <c r="H6" s="4" t="str">
         <f>IF(OR(F8 = "UNPLAYED", F8 = "XXX"), F8, -1* F8)</f>
@@ -1680,8 +1680,8 @@
       <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
+      <c r="F7" s="3">
+        <v>-45</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
updated for jan 22 session
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="544" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47FC00E8-1281-4563-94C4-CA62B8F806BC}"/>
+  <xr:revisionPtr revIDLastSave="548" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C33D93C-FDA3-479F-94C7-185A74F81F28}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="69">
   <si>
     <t>manler</t>
   </si>
@@ -906,7 +906,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -981,9 +981,9 @@
         <f>IF(OR(B8 = "UNPLAYED", B8 = "XXX"), B8, -1* B8)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="I2" s="1" t="str">
+      <c r="I2" s="1">
         <f>IF(OR(B9 = "UNPLAYED", B9 = "XXX"), B9, -1* B9)</f>
-        <v>UNPLAYED</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1" t="str">
         <f>IF(OR(B10 = "UNPLAYED", B10 = "XXX"), B10, -1* B10)</f>
@@ -1016,9 +1016,9 @@
         <f>IF(OR(C6 = "UNPLAYED", C6 = "XXX"), C6, -1* C6)</f>
         <v>-55</v>
       </c>
-      <c r="G3" s="1" t="str">
+      <c r="G3" s="1">
         <f>IF(OR(C7 = "UNPLAYED", C7 = "XXX"), C7, -1* C7)</f>
-        <v>UNPLAYED</v>
+        <v>-50</v>
       </c>
       <c r="H3" s="1" t="str">
         <f>IF(OR(C8 = "UNPLAYED", C8 = "XXX"), C8, -1* C8)</f>
@@ -1151,9 +1151,9 @@
         <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J6" s="1" t="str">
+      <c r="J6" s="1">
         <f>IF(OR(F10 = "UNPLAYED", F10 = "XXX"), F10, -1* F10)</f>
-        <v>UNPLAYED</v>
+        <v>15</v>
       </c>
       <c r="K6" s="1" t="str">
         <f>IF(OR(F11 = "UNPLAYED", F11 = "XXX"), F11, -1* F11)</f>
@@ -1167,8 +1167,8 @@
       <c r="B7" s="3">
         <v>-10</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
+      <c r="C7" s="3">
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>4</v>
@@ -1241,8 +1241,8 @@
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
+      <c r="B9" s="3">
+        <v>-55</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -1265,9 +1265,9 @@
       <c r="I9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="4" t="str">
+      <c r="J9" s="4">
         <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
-        <v>UNPLAYED</v>
+        <v>-90</v>
       </c>
       <c r="K9" s="4">
         <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
@@ -1290,8 +1290,8 @@
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
+      <c r="F10" s="3">
+        <v>-15</v>
       </c>
       <c r="G10" s="3">
         <v>20</v>
@@ -1299,8 +1299,8 @@
       <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>4</v>
+      <c r="I10" s="3">
+        <v>90</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
updated for feb 12 session
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C33D93C-FDA3-479F-94C7-185A74F81F28}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49E23F8C-7DE2-46DC-948E-187D6497D9C0}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="69">
   <si>
     <t>manler</t>
   </si>
@@ -582,10 +582,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -906,7 +902,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1410,7 +1406,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1558,9 +1554,9 @@
         <f>IF(OR(D5 = "UNPLAYED", D5 = "XXX"), D5, -1* D5)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="F4" s="4" t="str">
+      <c r="F4" s="4">
         <f>IF(OR(D6 = "UNPLAYED", D6 = "XXX"), D6, -1* D6)</f>
-        <v>UNPLAYED</v>
+        <v>-100</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>IF(OR(D7 = "UNPLAYED", D7 = "XXX"), D7, -1* D7)</f>
@@ -1634,8 +1630,8 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
+      <c r="D6" s="3">
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
@@ -1773,9 +1769,9 @@
         <f>IF(OR(I10 = "UNPLAYED", I10 = "XXX"), I10, -1* I10)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="K9" s="4" t="str">
+      <c r="K9" s="4">
         <f>IF(OR(I11 = "UNPLAYED", I11 = "XXX"), I11, -1* I11)</f>
-        <v>UNPLAYED</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1"/>
     </row>
@@ -1841,8 +1837,8 @@
       <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>4</v>
+      <c r="I11" s="3">
+        <v>0</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
updated for feb19 session
</commit_message>
<xml_diff>
--- a/static/jpFlicksSeason2.xlsx
+++ b/static/jpFlicksSeason2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09258977402b9a53/Desktop/COOP/futureMath/personalWebsite/my-website/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="550" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49E23F8C-7DE2-46DC-948E-187D6497D9C0}"/>
+  <xr:revisionPtr revIDLastSave="551" documentId="8_{867DBCD6-7AF9-4EBF-899F-19C6CCA2DE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE9356E6-A232-44A3-B93C-904FC1C387E1}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{F2CC4DDF-27B6-4D19-B743-3CECDC910C25}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeGames" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="69">
   <si>
     <t>manler</t>
   </si>
@@ -901,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D929F0-B3DC-465A-80A7-6440F9A84DDB}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -1405,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EF8B2E-F019-48DD-B57E-84981A9F67DB}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1651,9 +1651,9 @@
         <f>IF(OR(F9 = "UNPLAYED", F9 = "XXX"), F9, -1* F9)</f>
         <v>UNPLAYED</v>
       </c>
-      <c r="J6" s="1" t="str">
+      <c r="J6" s="1">
         <f>IF(OR(F10 = "UNPLAYED", F10 = "XXX"), F10, -1* F10)</f>
-        <v>UNPLAYED</v>
+        <v>-100</v>
       </c>
       <c r="K6" s="1" t="str">
         <f>IF(OR(F11 = "UNPLAYED", F11 = "XXX"), F11, -1* F11)</f>
@@ -1791,8 +1791,8 @@
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
+      <c r="F10" s="3">
+        <v>100</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>4</v>

</xml_diff>